<commit_message>
Revise Spare Part V2
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/SparePartRequestSheetIPO.xlsx
+++ b/bin/Debug/Template/SparePartRequestSheetIPO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT-Project\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783BEBE-DD6F-4A72-A3CB-744B20D9E2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4169E537-2939-4E85-B661-07E7B26B8DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BBFB412F-6E2A-4F5D-8DDF-BCB1C8845C69}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Document Nº:</t>
   </si>
@@ -73,34 +73,7 @@
     <t>New Unit Price</t>
   </si>
   <si>
-    <t>LeadTime</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Fatory Manager</t>
-  </si>
-  <si>
-    <t>Manager/Ast.Mgr/SV</t>
-  </si>
-  <si>
-    <t>Request</t>
-  </si>
-  <si>
-    <t>Date:……/……..../………...</t>
-  </si>
-  <si>
-    <t>Signature</t>
-  </si>
-  <si>
-    <t>………………………………………………………………….</t>
-  </si>
-  <si>
-    <t>……………………………………………………………</t>
-  </si>
-  <si>
-    <t>……………………………………………………..</t>
   </si>
   <si>
     <t>Spare Part Unit Price Request (IPO)</t>
@@ -192,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -252,15 +225,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -296,27 +260,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -336,9 +285,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,10 +313,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -382,13 +325,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -402,43 +345,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical style="thin">
-          <color rgb="FF000000"/>
-        </vertical>
-        <horizontal style="thin">
-          <color rgb="FF000000"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <b val="0"/>
@@ -1550,20 +1457,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78277B55-40C9-44DD-9957-331E1E3EEEEF}" name="PrintForm" displayName="PrintForm" ref="A3:K4" insertRow="1" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A3:K4" xr:uid="{82AADA1B-A3F6-4D5A-9B6D-24C3D1153767}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F252EC0F-AA97-46A5-84A8-11D8474EEEBF}" name="Code" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1164D89B-C5E9-49D4-BC69-EFED51D5606F}" name="Part Number" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{512A3FEF-9335-4251-90FE-39A702AD8547}" name="Part Name" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{2B65F916-A3FB-4E7C-A6CF-9E39B12D591A}" name="Machine Name" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{97D271A3-F359-4954-AD16-22CA66208BE5}" name="Supplier" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{245AA6F7-F3DA-4E23-ABB5-96CFC00A7EE4}" name="Maker" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{62E00F1B-299D-474C-BF74-367D6115D293}" name="Qty" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{E0ABF327-44D9-4CAA-BA48-9A2CEDF273E5}" name="Unit Price" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="10" xr3:uid="{65840F35-6DB8-417A-8061-0540AB30AEEE}" name="Amount" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{45E8E37F-A983-4B83-8BD0-97CD2AA7E98A}" name="New Unit Price" dataDxfId="2" totalsRowDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{C0DCCB59-C8E6-45A1-B7C5-1751682DE40C}" name="LeadTime" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78277B55-40C9-44DD-9957-331E1E3EEEEF}" name="PrintForm" displayName="PrintForm" ref="A3:J4" insertRow="1" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:J4" xr:uid="{82AADA1B-A3F6-4D5A-9B6D-24C3D1153767}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{F252EC0F-AA97-46A5-84A8-11D8474EEEBF}" name="Code" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{1164D89B-C5E9-49D4-BC69-EFED51D5606F}" name="Part Number" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{512A3FEF-9335-4251-90FE-39A702AD8547}" name="Part Name" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{2B65F916-A3FB-4E7C-A6CF-9E39B12D591A}" name="Machine Name" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{97D271A3-F359-4954-AD16-22CA66208BE5}" name="Supplier" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{245AA6F7-F3DA-4E23-ABB5-96CFC00A7EE4}" name="Maker" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{62E00F1B-299D-474C-BF74-367D6115D293}" name="Qty" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{E0ABF327-44D9-4CAA-BA48-9A2CEDF273E5}" name="Unit Price" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{65840F35-6DB8-417A-8061-0540AB30AEEE}" name="Amount" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{45E8E37F-A983-4B83-8BD0-97CD2AA7E98A}" name="New Unit Price" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1867,10 +1773,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883FEBF2-0291-4497-8498-5E7B5954CAD9}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,30 +1790,29 @@
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>21</v>
+    <row r="1" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2" t="s">
@@ -1915,7 +1820,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1946,111 +1851,82 @@
       <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24">
         <f>SUM(PrintForm[Amount])</f>
         <v>0</v>
       </c>
-      <c r="J5" s="27"/>
+      <c r="J5" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="16"/>
-      <c r="I7" s="16" t="s">
-        <v>15</v>
-      </c>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="15"/>
+      <c r="I7" s="15"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+    <row r="8" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="15"/>
-      <c r="I9" s="16" t="s">
-        <v>17</v>
-      </c>
+    <row r="9" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="14"/>
+      <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="H11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+    <row r="10" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
     </row>
-    <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>